<commit_message>
midway through Realm reporting - waiting on Fusion support for realm report with context_names
</commit_message>
<xml_diff>
--- a/STAAS-Fleet-2025-02.xlsx
+++ b/STAAS-Fleet-2025-02.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -680,6 +680,198 @@
         <v>327362483176</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2025-02-07 13:41</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>pstg-fa-03</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" t="n">
+        <v>102402176</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" t="n">
+        <v>107961344</v>
+      </c>
+      <c r="I6" t="n">
+        <v>1</v>
+      </c>
+      <c r="J6" t="n">
+        <v>5559168</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" t="n">
+        <v>1111537536204800</v>
+      </c>
+      <c r="M6" t="n">
+        <v>107961344</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2025-02-07 13:41</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>pstg-fa-02</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>4.13294045762392</v>
+      </c>
+      <c r="D7" t="n">
+        <v>142350152779</v>
+      </c>
+      <c r="E7" t="n">
+        <v>58263161536</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.999815000270004</v>
+      </c>
+      <c r="H7" t="n">
+        <v>327266564890</v>
+      </c>
+      <c r="I7" t="n">
+        <v>22251.60979597833</v>
+      </c>
+      <c r="J7" t="n">
+        <v>126653250575</v>
+      </c>
+      <c r="K7" t="n">
+        <v>1029782972928</v>
+      </c>
+      <c r="L7" t="n">
+        <v>5566402572320768</v>
+      </c>
+      <c r="M7" t="n">
+        <v>327266564890</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2025-02-07 15:22</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>pstg-fa-03</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" t="n">
+        <v>102402176</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" t="n">
+        <v>107961344</v>
+      </c>
+      <c r="I8" t="n">
+        <v>1</v>
+      </c>
+      <c r="J8" t="n">
+        <v>5559168</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>1111537536204800</v>
+      </c>
+      <c r="M8" t="n">
+        <v>107961344</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2025-02-07 15:22</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>pstg-fa-02</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>4.134110249036264</v>
+      </c>
+      <c r="D9" t="n">
+        <v>142260835620</v>
+      </c>
+      <c r="E9" t="n">
+        <v>58262194555</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.9998149961214116</v>
+      </c>
+      <c r="H9" t="n">
+        <v>327178912324</v>
+      </c>
+      <c r="I9" t="n">
+        <v>22257.41077400217</v>
+      </c>
+      <c r="J9" t="n">
+        <v>126655882149</v>
+      </c>
+      <c r="K9" t="n">
+        <v>1029806065664</v>
+      </c>
+      <c r="L9" t="n">
+        <v>5566402572320768</v>
+      </c>
+      <c r="M9" t="n">
+        <v>327178912324</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>